<commit_message>
INFORME FINAL 02 - RESONANCIA
</commit_message>
<xml_diff>
--- a/2. CIRCUITOS RESONANTES/INFORME FINAL/mediciones_experimentales.xlsx
+++ b/2. CIRCUITOS RESONANTES/INFORME FINAL/mediciones_experimentales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bremdows\UNSAAC\SEMESTRE VIII\CIRCUITOS ELECTRONICOS III\laboratorio\2. CIRCUITOS RESONANTES\INFORME FINAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNSAAC\SEMESTRE VIII\CIRCUITOS ELECTRÓNICOS IIII\laboratorio\2. CIRCUITOS RESONANTES\INFORME FINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D420C75C-C7DD-4433-A143-329B3E36606B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595E35D5-5E2C-45C1-BFE0-927943829B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{9EA46989-2BD2-4071-B6ED-0B644DE0A24C}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{9EA46989-2BD2-4071-B6ED-0B644DE0A24C}"/>
   </bookViews>
   <sheets>
     <sheet name="Circuito Serie" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,12 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>F [Hz]</t>
-  </si>
-  <si>
-    <t>Vo [V]</t>
   </si>
   <si>
     <t>Io [mA]</t>
@@ -65,13 +60,30 @@
   <si>
     <t>2.9M</t>
   </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,37 +122,23 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -174,6 +172,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Io [mA]</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> -  Frecuencia [Hz]</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -214,7 +242,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Circuito Serie'!$C$2</c:f>
+              <c:f>'Circuito Serie'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -387,7 +415,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Circuito Serie'!$C$2:$C$45</c:f>
+              <c:f>'Circuito Serie'!$B$2:$B$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="44"/>
@@ -1281,15 +1309,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>617220</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>428626</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1614,875 +1642,896 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF693FA-A3D3-4031-B60A-9597932931C7}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <f>0.009</f>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1">
+      <c r="J2">
         <f>1/(2*PI()*SQRT(5*10^-6*10*10^-3))</f>
         <v>711.76254341717708</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="B3" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <f>5.6*10^-6</f>
+        <v>5.5999999999999997E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>20</v>
       </c>
-      <c r="C4">
+      <c r="B4" s="3">
         <v>4.01</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>50</v>
       </c>
-      <c r="C5">
+      <c r="B5" s="3">
         <v>4.03</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>100</v>
       </c>
-      <c r="C6">
+      <c r="B6" s="3">
         <v>4.12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <f>A6 + 100</f>
         <v>200</v>
       </c>
-      <c r="C7">
+      <c r="B7" s="3">
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <f t="shared" ref="A8:A12" si="0">A7 + 100</f>
         <v>300</v>
       </c>
-      <c r="C8">
+      <c r="B8" s="3">
         <v>4.22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="C9">
+      <c r="B9" s="3">
         <v>4.25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="C10">
+      <c r="B10" s="3">
         <v>4.37</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
-      <c r="C11">
+      <c r="B11" s="3">
         <v>4.49</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="C12">
+      <c r="B12" s="3">
         <v>4.6399999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>711</v>
       </c>
-      <c r="C13">
+      <c r="B13" s="3">
         <v>4.72</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>850</v>
       </c>
-      <c r="C14">
+      <c r="B14" s="3">
         <v>4.96</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>950</v>
       </c>
-      <c r="C15">
+      <c r="B15" s="3">
         <v>5.09</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>1000</v>
       </c>
-      <c r="C16">
+      <c r="B16" s="3">
         <v>5.16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>1200</v>
       </c>
-      <c r="C17">
+      <c r="B17" s="3">
         <v>5.53</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>2000</v>
       </c>
-      <c r="C18">
+      <c r="B18" s="3">
         <v>7.47</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>2500</v>
       </c>
-      <c r="C19">
+      <c r="B19" s="3">
         <v>8.73</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>3500</v>
       </c>
-      <c r="C20">
+      <c r="B20" s="3">
         <v>11.45</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>5000</v>
       </c>
-      <c r="C21">
+      <c r="B21" s="3">
         <v>15.72</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>6000</v>
       </c>
-      <c r="C22">
+      <c r="B22" s="3">
         <v>18.649999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>7000</v>
       </c>
-      <c r="C23">
+      <c r="B23" s="3">
         <v>21.55</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>8000</v>
       </c>
-      <c r="C24">
+      <c r="B24" s="3">
         <v>24.48</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>9000</v>
       </c>
-      <c r="C25">
+      <c r="B25" s="3">
         <v>27.42</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>10000</v>
       </c>
-      <c r="C26">
+      <c r="B26" s="3">
         <v>30.39</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>20000</v>
       </c>
-      <c r="C27">
+      <c r="B27" s="3">
         <v>60.51</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>30000</v>
       </c>
-      <c r="C28">
+      <c r="B28" s="3">
         <v>91.98</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>40000</v>
       </c>
-      <c r="C29">
+      <c r="B29" s="3">
         <v>126.41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>50000</v>
       </c>
-      <c r="C30">
+      <c r="B30" s="3">
         <v>160.55000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>60000</v>
       </c>
-      <c r="C31">
+      <c r="B31" s="3">
         <v>203.45</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>70000</v>
       </c>
-      <c r="C32">
+      <c r="B32" s="3">
         <v>252.24</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>80000</v>
       </c>
-      <c r="C33">
+      <c r="B33" s="3">
         <v>315.72000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>90000</v>
       </c>
-      <c r="C34">
+      <c r="B34" s="3">
         <v>383.77</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>100000</v>
       </c>
-      <c r="C35">
+      <c r="B35" s="3">
         <v>462.67</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>200000</v>
       </c>
-      <c r="C36">
+      <c r="B36" s="3">
         <v>305.25</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>300000</v>
       </c>
-      <c r="C37">
+      <c r="B37" s="3">
         <v>104.68</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>400000</v>
       </c>
-      <c r="C38">
+      <c r="B38" s="3">
         <v>43.47</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>500000</v>
       </c>
-      <c r="C39">
+      <c r="B39" s="3">
         <v>15.17</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>600000</v>
       </c>
-      <c r="C40">
+      <c r="B40" s="3">
         <v>5.05</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>700000</v>
       </c>
-      <c r="C41">
+      <c r="B41" s="3">
         <v>9.2799999999999994</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>800000</v>
       </c>
-      <c r="C42">
+      <c r="B42" s="3">
         <v>24.5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>900000</v>
       </c>
-      <c r="C43">
+      <c r="B43" s="3">
         <v>48.19</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>1000000</v>
       </c>
+      <c r="B44" s="3">
+        <v>56.48</v>
+      </c>
       <c r="C44">
-        <v>56.48</v>
-      </c>
-      <c r="D44">
         <v>56.13</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>2000000</v>
       </c>
-      <c r="C45">
+      <c r="B45" s="3">
         <v>4.7699999999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="5">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>3000000</v>
       </c>
-      <c r="C46">
+      <c r="B46" s="3">
         <v>4.67</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9524711-997D-4542-BF7C-1F5579143095}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="B3" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>20</v>
       </c>
-      <c r="C4">
+      <c r="B4" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>50</v>
       </c>
-      <c r="C5">
+      <c r="B5" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>100</v>
       </c>
-      <c r="C6">
+      <c r="B6" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <f>A6 + 100</f>
         <v>200</v>
       </c>
-      <c r="C7">
+      <c r="B7" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <f t="shared" ref="A8:A12" si="0">A7 + 100</f>
         <v>300</v>
       </c>
-      <c r="C8">
+      <c r="B8" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="C9">
+      <c r="B9" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="C10">
+      <c r="B10" s="3">
         <v>2.09</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
-      <c r="C11">
+      <c r="B11" s="3">
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="C12">
+      <c r="B12" s="3">
         <v>2.9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>711</v>
       </c>
-      <c r="C13">
+      <c r="B13" s="3">
         <v>2.95</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>850</v>
       </c>
-      <c r="C14">
+      <c r="B14" s="3">
         <v>3.54</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>950</v>
       </c>
-      <c r="C15">
+      <c r="B15" s="3">
         <v>3.96</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>1000</v>
       </c>
-      <c r="C16">
+      <c r="B16" s="3">
         <v>4.17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>1200</v>
       </c>
-      <c r="C17">
+      <c r="B17" s="3">
         <v>5.01</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>2000</v>
       </c>
-      <c r="C18">
+      <c r="B18" s="3">
         <v>8.44</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>2500</v>
       </c>
-      <c r="C19">
+      <c r="B19" s="3">
         <v>10.58</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>3500</v>
       </c>
-      <c r="C20">
+      <c r="B20" s="3">
         <v>14.91</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>5000</v>
       </c>
-      <c r="C21">
+      <c r="B21" s="3">
         <v>21.45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>6000</v>
       </c>
-      <c r="C22">
+      <c r="B22" s="3">
         <v>25.84</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>7000</v>
       </c>
-      <c r="C23">
+      <c r="B23" s="3">
         <v>30.22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>8000</v>
       </c>
-      <c r="C24">
+      <c r="B24" s="3">
         <v>34.61</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>9000</v>
       </c>
-      <c r="C25">
+      <c r="B25" s="3">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>10000</v>
       </c>
-      <c r="C26">
+      <c r="B26" s="3">
         <v>43.38</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>20000</v>
       </c>
-      <c r="C27">
+      <c r="B27" s="3">
         <v>86.49</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>30000</v>
       </c>
-      <c r="C28">
+      <c r="B28" s="3">
         <v>128.38</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>40000</v>
       </c>
-      <c r="C29">
+      <c r="B29" s="3">
         <v>168.6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>50000</v>
       </c>
-      <c r="C30">
+      <c r="B30" s="3">
         <v>206.73</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>60000</v>
       </c>
-      <c r="C31">
+      <c r="B31" s="3">
         <v>243.43</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>70000</v>
       </c>
-      <c r="C32">
+      <c r="B32" s="3">
         <v>278.23</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>80000</v>
       </c>
-      <c r="C33">
+      <c r="B33" s="3">
         <v>311.22000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>90000</v>
       </c>
-      <c r="C34">
+      <c r="B34" s="3">
         <v>342.45</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>100000</v>
       </c>
-      <c r="C35">
+      <c r="B35" s="3">
         <v>371.98</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>200000</v>
       </c>
-      <c r="C36">
+      <c r="B36" s="3">
         <v>573.69000000000005</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>300000</v>
       </c>
-      <c r="C37">
+      <c r="B37" s="3">
         <v>684.1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>400000</v>
       </c>
-      <c r="C38">
+      <c r="B38" s="3">
         <v>783.61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>500000</v>
       </c>
-      <c r="C39">
+      <c r="B39" s="3">
         <v>969.52</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>600000</v>
       </c>
-      <c r="C40">
+      <c r="B40" s="3">
         <v>1192.3</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>700000</v>
       </c>
-      <c r="C41">
+      <c r="B41" s="3">
         <v>1486.3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>800000</v>
       </c>
-      <c r="C42">
+      <c r="B42" s="3">
         <v>1933.1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>900000</v>
       </c>
-      <c r="C43">
+      <c r="B43" s="3">
         <v>2548.3000000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>1000000</v>
       </c>
-      <c r="C44">
+      <c r="B44" s="3">
         <v>2679.5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>2000000</v>
       </c>
-      <c r="C45">
+      <c r="B45" s="3">
         <v>1548.5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="5">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <f>2.1*10^6</f>
         <v>2100000</v>
       </c>
-      <c r="C46">
+      <c r="B46" s="3">
         <v>1144.2</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="5">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <f>2.2*10^6</f>
         <v>2200000</v>
       </c>
-      <c r="C47">
+      <c r="B47" s="3">
         <v>720.2</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="5">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <f>2.3*10^6</f>
         <v>2300000</v>
       </c>
-      <c r="C48">
+      <c r="B48" s="3">
         <v>351.9</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="5">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <f>2.4*10^6</f>
         <v>2400000</v>
       </c>
-      <c r="C49">
+      <c r="B49" s="3">
         <v>177.01</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="5">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <f>2.5*10^6</f>
         <v>2500000</v>
       </c>
-      <c r="C50">
+      <c r="B50" s="3">
         <v>104.5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="3">
+        <v>70.099999999999994</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C51">
-        <v>70.099999999999994</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="B52" s="3">
+        <v>51.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C52">
-        <v>51.6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="B53" s="3">
+        <v>40.6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C53">
-        <v>40.6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54">
+      <c r="B54" s="3">
         <v>33.700000000000003</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
         <v>3</v>
       </c>
-      <c r="C55">
+      <c r="B55" s="3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>